<commit_message>
UPDATE MENU FILE - CREATE TASKS REMINDER
</commit_message>
<xml_diff>
--- a/MENU/PROPOSAL/FYP - TIMELINE.xlsx
+++ b/MENU/PROPOSAL/FYP - TIMELINE.xlsx
@@ -70,7 +70,7 @@
     <t>5-12/7/2020</t>
   </si>
   <si>
-    <t>WEEK 1</t>
+    <t>WEEK 1-3</t>
   </si>
   <si>
     <t>→ 分工 design</t>
@@ -79,7 +79,7 @@
     <t>13-19/7/2020</t>
   </si>
   <si>
-    <t>WEEK 2</t>
+    <t>WEEK 4</t>
   </si>
   <si>
     <t>INTERIM PRESENTATION</t>
@@ -91,7 +91,7 @@
     <t>20/7/2020</t>
   </si>
   <si>
-    <t>WEEK 3-5</t>
+    <t>WEEK 5</t>
   </si>
   <si>
     <t xml:space="preserve">→ ANALYSIS </t>
@@ -186,9 +186,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -255,6 +255,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -262,7 +269,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -276,8 +312,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,51 +322,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,6 +367,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -366,39 +375,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="42">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,12 +443,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -461,187 +455,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,6 +750,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -790,50 +799,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -848,6 +813,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -856,10 +850,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -868,137 +862,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1086,9 +1080,6 @@
     <xf numFmtId="58" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1122,9 +1113,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1134,43 +1122,37 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1513,7 +1495,7 @@
   <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -1623,45 +1605,45 @@
       <c r="C8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="31"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="23"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="32"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="39" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="10">
@@ -1672,82 +1654,82 @@
       </c>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="41"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43" t="s">
+      <c r="D11" s="40"/>
+      <c r="E11" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="44"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="23"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="44"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="10">
         <v>21</v>
       </c>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="48"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="44"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="49"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="23"/>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="47" t="s">
         <v>41</v>
       </c>
       <c r="G16" s="3">
@@ -1756,32 +1738,32 @@
       <c r="H16" s="15"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="48"/>
-      <c r="C17" s="48" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="50" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="51"/>
+      <c r="F17" s="47"/>
       <c r="G17" s="3"/>
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="50" t="s">
         <v>48</v>
       </c>
       <c r="G18" s="10">
@@ -1790,52 +1772,52 @@
       <c r="H18" s="15"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="37"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="53" t="s">
+      <c r="B19" s="36"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="56"/>
+      <c r="F19" s="52"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="57"/>
-      <c r="C20" s="57" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="53" t="s">
+      <c r="D20" s="43"/>
+      <c r="E20" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="56"/>
+      <c r="F20" s="52"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="58"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="54"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="59"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="55"/>
       <c r="G22" s="23">
         <v>70</v>
       </c>

</xml_diff>